<commit_message>
Updated Code and Charts and Implemented Pie chart
</commit_message>
<xml_diff>
--- a/HOMA_NV_Metrics/keywords/TC001.xlsx
+++ b/HOMA_NV_Metrics/keywords/TC001.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse Neon\NeoNEclipsE\HOMA_NV_Metrics\keywords\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nkarthikeyan\git\iTF_HOMA\HOMA_NV_Metrics\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="215">
   <si>
     <t>Keyword</t>
   </si>
@@ -273,18 +273,9 @@
     <t>Male</t>
   </si>
   <si>
-    <t>txtdob</t>
-  </si>
-  <si>
-    <t>//*[@id='userFormOtherInfo']/div/div/div/div[2]/div[1]/div/div/div/div/div[3]/div/div[12]</t>
-  </si>
-  <si>
     <t>ddlNakshatra</t>
   </si>
   <si>
-    <t xml:space="preserve">Krittikai [Rishabham] (Kaarttkai) </t>
-  </si>
-  <si>
     <t>txtworkphone</t>
   </si>
   <si>
@@ -342,12 +333,6 @@
     <t>Enter Username</t>
   </si>
   <si>
-    <t>Select Dob</t>
-  </si>
-  <si>
-    <t>Select date</t>
-  </si>
-  <si>
     <t>Enter Work Phone No.</t>
   </si>
   <si>
@@ -372,12 +357,6 @@
     <t>clickById</t>
   </si>
   <si>
-    <t>//*[@id='userFormOtherInfo']/div/div/div/div[2]/div[1]/div/label</t>
-  </si>
-  <si>
-    <t>To close the D.O.B</t>
-  </si>
-  <si>
     <t>Enter Address</t>
   </si>
   <si>
@@ -510,6 +489,174 @@
     <t>TC030</t>
   </si>
   <si>
+    <t>TC034</t>
+  </si>
+  <si>
+    <t>TC035</t>
+  </si>
+  <si>
+    <t>TC036</t>
+  </si>
+  <si>
+    <t>TC037</t>
+  </si>
+  <si>
+    <t>TC038</t>
+  </si>
+  <si>
+    <t>TC039</t>
+  </si>
+  <si>
+    <t>TC040</t>
+  </si>
+  <si>
+    <t>TC041</t>
+  </si>
+  <si>
+    <t>TC042</t>
+  </si>
+  <si>
+    <t>TC043</t>
+  </si>
+  <si>
+    <t>TC044</t>
+  </si>
+  <si>
+    <t>TC045</t>
+  </si>
+  <si>
+    <t>TC046</t>
+  </si>
+  <si>
+    <t>TC047</t>
+  </si>
+  <si>
+    <t>TC048</t>
+  </si>
+  <si>
+    <t>TC049</t>
+  </si>
+  <si>
+    <t>TC050</t>
+  </si>
+  <si>
+    <t>TC051</t>
+  </si>
+  <si>
+    <t>TC052</t>
+  </si>
+  <si>
+    <t>TC053</t>
+  </si>
+  <si>
+    <t>TC054</t>
+  </si>
+  <si>
+    <t>TC055</t>
+  </si>
+  <si>
+    <t>TC056</t>
+  </si>
+  <si>
+    <t>TC057</t>
+  </si>
+  <si>
+    <t>TC058</t>
+  </si>
+  <si>
+    <t>TC059</t>
+  </si>
+  <si>
+    <t>TC060</t>
+  </si>
+  <si>
+    <t>TC061</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Test Procedure</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Test case Type</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Validation Message</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>Other Information</t>
+  </si>
+  <si>
+    <t>Login Information</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Profile Information</t>
+  </si>
+  <si>
+    <t>Testing Type</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Non-Functional</t>
+  </si>
+  <si>
+    <t>3 - Medium</t>
+  </si>
+  <si>
+    <t>4 - Low</t>
+  </si>
+  <si>
+    <t>1 - Critical</t>
+  </si>
+  <si>
+    <t>2 - High</t>
+  </si>
+  <si>
+    <t>Not Known</t>
+  </si>
+  <si>
+    <t>Enter Gothra</t>
+  </si>
+  <si>
+    <t>txtGotra</t>
+  </si>
+  <si>
+    <t>we123</t>
+  </si>
+  <si>
     <t>TC031</t>
   </si>
   <si>
@@ -517,175 +664,12 @@
   </si>
   <si>
     <t>TC033</t>
-  </si>
-  <si>
-    <t>TC034</t>
-  </si>
-  <si>
-    <t>TC035</t>
-  </si>
-  <si>
-    <t>TC036</t>
-  </si>
-  <si>
-    <t>TC037</t>
-  </si>
-  <si>
-    <t>TC038</t>
-  </si>
-  <si>
-    <t>TC039</t>
-  </si>
-  <si>
-    <t>TC040</t>
-  </si>
-  <si>
-    <t>TC041</t>
-  </si>
-  <si>
-    <t>TC042</t>
-  </si>
-  <si>
-    <t>TC043</t>
-  </si>
-  <si>
-    <t>TC044</t>
-  </si>
-  <si>
-    <t>TC045</t>
-  </si>
-  <si>
-    <t>TC046</t>
-  </si>
-  <si>
-    <t>TC047</t>
-  </si>
-  <si>
-    <t>TC048</t>
-  </si>
-  <si>
-    <t>TC049</t>
-  </si>
-  <si>
-    <t>TC050</t>
-  </si>
-  <si>
-    <t>TC051</t>
-  </si>
-  <si>
-    <t>TC052</t>
-  </si>
-  <si>
-    <t>TC053</t>
-  </si>
-  <si>
-    <t>TC054</t>
-  </si>
-  <si>
-    <t>TC055</t>
-  </si>
-  <si>
-    <t>TC056</t>
-  </si>
-  <si>
-    <t>TC057</t>
-  </si>
-  <si>
-    <t>TC058</t>
-  </si>
-  <si>
-    <t>TC059</t>
-  </si>
-  <si>
-    <t>TC060</t>
-  </si>
-  <si>
-    <t>TC061</t>
-  </si>
-  <si>
-    <t>TC062</t>
-  </si>
-  <si>
-    <t>TC063</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Test Scenario</t>
-  </si>
-  <si>
-    <t>Test Procedure</t>
-  </si>
-  <si>
-    <t>Module Name</t>
-  </si>
-  <si>
-    <t>Test case Type</t>
-  </si>
-  <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>Validation Message</t>
-  </si>
-  <si>
-    <t>User Management</t>
-  </si>
-  <si>
-    <t>Other Information</t>
-  </si>
-  <si>
-    <t>Login Information</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>Profile Information</t>
-  </si>
-  <si>
-    <t>Testing Type</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t>Non-Functional</t>
-  </si>
-  <si>
-    <t>3 - Medium</t>
-  </si>
-  <si>
-    <t>4 - Low</t>
-  </si>
-  <si>
-    <t>1 - Critical</t>
-  </si>
-  <si>
-    <t>2 - High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -829,10 +813,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,53 +1120,52 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q470"/>
+  <dimension ref="A1:O469"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="92.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="109.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="54.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="59.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="19.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="92.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="54.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="59.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>211</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>0</v>
@@ -1196,43 +1177,41 @@
         <v>1</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I2" s="9" t="s">
         <v>21</v>
       </c>
@@ -1244,34 +1223,32 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P2" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G3" s="10">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1283,34 +1260,32 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P3" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1322,34 +1297,32 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P4" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G5" s="10">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1361,34 +1334,32 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P5" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1400,34 +1371,32 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P6" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G7" s="10">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I7" s="9" t="s">
         <v>21</v>
       </c>
@@ -1439,34 +1408,32 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P7" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G8" s="10">
+        <v>4</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1480,34 +1447,32 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P8" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G9" s="10">
+        <v>4</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
       <c r="I9" s="9" t="s">
         <v>21</v>
       </c>
@@ -1519,34 +1484,32 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P9" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I10" s="9" t="s">
         <v>21</v>
       </c>
@@ -1558,34 +1521,32 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P10" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G11" s="10">
+        <v>3</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I11" s="9" t="s">
         <v>27</v>
       </c>
@@ -1599,34 +1560,32 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P11" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G12" s="10">
+        <v>3</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1640,34 +1599,32 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P12" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G13" s="10">
+        <v>3</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I13" s="9" t="s">
         <v>27</v>
       </c>
@@ -1681,34 +1638,32 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P13" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I14" s="9" t="s">
         <v>29</v>
       </c>
@@ -1722,34 +1677,32 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P14" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G15" s="10">
+        <v>2</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I15" s="9" t="s">
         <v>27</v>
       </c>
@@ -1763,34 +1716,32 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P15" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I16" s="9" t="s">
         <v>29</v>
       </c>
@@ -1804,34 +1755,32 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P16" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I17" s="9" t="s">
         <v>27</v>
       </c>
@@ -1845,34 +1794,32 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P17" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I18" s="9" t="s">
         <v>29</v>
       </c>
@@ -1886,34 +1833,32 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P18" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I19" s="9" t="s">
         <v>54</v>
       </c>
@@ -1927,34 +1872,32 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P19" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I20" s="9" t="s">
         <v>29</v>
       </c>
@@ -1968,34 +1911,32 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P20" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I21" s="9" t="s">
         <v>27</v>
       </c>
@@ -2009,34 +1950,32 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P21" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
         <v>75</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G22" s="10">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I22" s="9" t="s">
         <v>29</v>
       </c>
@@ -2050,34 +1989,32 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P22" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G23" s="10">
+        <v>3</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I23" s="9" t="s">
         <v>27</v>
       </c>
@@ -2085,40 +2022,38 @@
         <v>61</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P23" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>75</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G24" s="10">
+        <v>3</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I24" s="9" t="s">
         <v>29</v>
       </c>
@@ -2132,34 +2067,32 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P24" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G25" s="10">
+        <v>4</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I25" s="9" t="s">
         <v>27</v>
       </c>
@@ -2173,34 +2106,32 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P25" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q25" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G26" s="10">
+        <v>3</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I26" s="9" t="s">
         <v>29</v>
       </c>
@@ -2214,34 +2145,32 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P26" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q26" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G27" s="10">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I27" s="9" t="s">
         <v>69</v>
       </c>
@@ -2255,34 +2184,32 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P27" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G28" s="10">
+        <v>3</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="I28" s="9" t="s">
         <v>27</v>
       </c>
@@ -2296,34 +2223,32 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P28" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q28" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G29" s="10">
+        <v>2</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I29" s="9" t="s">
         <v>27</v>
       </c>
@@ -2337,34 +2262,32 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P29" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q29" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G30" s="10">
+        <v>2</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I30" s="9" t="s">
         <v>6</v>
       </c>
@@ -2376,34 +2299,32 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P30" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q30" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G31" s="10">
+        <v>2</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I31" s="9" t="s">
         <v>69</v>
       </c>
@@ -2417,192 +2338,188 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P31" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q31" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G32" s="10">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I32" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K32" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P32" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q32" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G33" s="10">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I33" s="9" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="K33" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P33" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G34" s="10">
+        <v>3</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="I34" s="9" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="10"/>
+      <c r="K34" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P34" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I35" s="9" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="L35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P35" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G36" s="10">
+        <v>3</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="I36" s="9" t="s">
         <v>27</v>
       </c>
@@ -2616,34 +2533,32 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P36" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q36" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
         <v>75</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G37" s="10">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I37" s="9" t="s">
         <v>29</v>
       </c>
@@ -2657,34 +2572,32 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P37" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G38" s="10">
+        <v>3</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
       <c r="I38" s="9" t="s">
         <v>27</v>
       </c>
@@ -2692,168 +2605,158 @@
         <v>91</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P38" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q38" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G39" s="10">
+        <v>2</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I39" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P39" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G40" s="10">
+        <v>4</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I40" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P40" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q40" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G41" s="10">
+        <v>3</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I41" s="9" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P41" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q41" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G42" s="10">
+        <v>2</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="I42" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>98</v>
@@ -2862,600 +2765,570 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P42" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q42" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="G43" s="10">
+        <v>2</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I43" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
+      <c r="L43" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P43" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q43" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G44" s="10">
+        <v>2</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I44" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P44" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q44" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G45" s="10">
+        <v>3</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I45" s="9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="K45" s="4"/>
-      <c r="L45" s="4" t="s">
-        <v>102</v>
-      </c>
+      <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P45" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q45" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G46" s="10">
+        <v>2</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I46" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P46" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q46" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G47" s="10">
+        <v>1</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I47" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K47" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P47" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q47" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G48" s="10">
+        <v>1</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I48" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P48" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q48" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G49" s="10">
+        <v>1</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I49" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P49" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q49" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G50" s="10">
+        <v>1</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I50" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P50" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q50" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G51" s="10">
+        <v>3</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I51" s="9" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P51" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q51" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G52" s="10">
+        <v>3</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I52" s="9" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>125</v>
+        <v>57</v>
+      </c>
+      <c r="K52" s="4">
+        <v>93781498314</v>
       </c>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P52" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q52" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G53" s="10">
+        <v>3</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I53" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K53" s="4">
-        <v>93781498314</v>
+        <v>61</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P53" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q53" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G54" s="10">
+        <v>3</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I54" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="K54" s="4">
+        <v>352523423</v>
       </c>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P54" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q54" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G55" s="10">
+        <v>3</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J55" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K55" s="4">
-        <v>352523423</v>
-      </c>
+      <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P55" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q55" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G56" s="10">
+        <v>3</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I56" s="9" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="K56" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="K56" s="4">
+        <v>97898786896</v>
+      </c>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P56" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q56" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G57" s="10">
+        <v>4</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I57" s="9" t="s">
         <v>27</v>
       </c>
@@ -3463,305 +3336,263 @@
         <v>88</v>
       </c>
       <c r="K57" s="4">
-        <v>97898786896</v>
+        <v>8979696978</v>
       </c>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P57" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q57" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G58" s="10">
+        <v>4</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I58" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="K58" s="4">
-        <v>8979696978</v>
+      <c r="K58" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P58" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q58" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G59" s="10">
+        <v>3</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I59" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P59" s="11">
-        <v>4</v>
-      </c>
-      <c r="Q59" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G60" s="10">
+        <v>3</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I60" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P60" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q60" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G61" s="10">
+        <v>3</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I61" s="9" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>127</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P61" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q61" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G62" s="10">
+        <v>3</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I62" s="9" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="K62" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P62" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q62" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="G63" s="10">
+        <v>2</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I63" s="9" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>132</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="K63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P63" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q63" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>195</v>
-      </c>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>214</v>
-      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-      <c r="I64" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="I64" s="9"/>
+      <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P64" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q64" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O64" s="4"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -3777,10 +3608,8 @@
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="5"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -3796,10 +3625,8 @@
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="5"/>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -3815,10 +3642,8 @@
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="5"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -3834,10 +3659,8 @@
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
-      <c r="P68" s="11"/>
-      <c r="Q68" s="5"/>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -3853,10 +3676,8 @@
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="5"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -3872,10 +3693,8 @@
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="5"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -3891,10 +3710,8 @@
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
-      <c r="P71" s="11"/>
-      <c r="Q71" s="5"/>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -3910,37 +3727,16 @@
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
       <c r="O72" s="4"/>
-      <c r="P72" s="11"/>
-      <c r="Q72" s="5"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
-      <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-      <c r="P73" s="11"/>
-      <c r="Q73" s="5"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J78" s="1"/>
-    </row>
-    <row r="470" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J470" s="1"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="469" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J469" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K59" r:id="rId1"/>
+    <hyperlink ref="K58" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>